<commit_message>
Start reworking Shiny test app to have sections inside tabs
</commit_message>
<xml_diff>
--- a/Pre-eclampsia_dataset_raw_and_processed/Pre_eclampsia_mice_rnasplice_results/multiqc/2024-08-21_general_statistics_dataset.xlsx
+++ b/Pre-eclampsia_dataset_raw_and_processed/Pre_eclampsia_mice_rnasplice_results/multiqc/2024-08-21_general_statistics_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Win_Ubuntu_shared\Pre-eclampsia_dataset_raw_and_processed\Pre_eclampsia_mice_rnasplice_results\multiqc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D05537-AEC8-44CF-AE32-602CAB218D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0F2668-F30A-4BDD-B3DA-4782BFD0F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="1" xr2:uid="{0D67E495-F5C7-481F-BA27-8860DF2F4FD3}"/>
   </bookViews>
@@ -691,12 +691,12 @@
   <dimension ref="A1:X49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+      <selection activeCell="D48" activeCellId="33" sqref="A4 D4 A6 D6 A10 D10 A1 D1 A12 D12 A16 D16 A18 D18 A22 D22 A24 D24 A28 D28 A30 D30 A34 D34 A36 D36 A40 D40 A42 D42 A46 D46 A48 D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" x14ac:dyDescent="0.45">
@@ -2796,10 +2796,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D69BE8D-618B-4D19-85AA-4129EEA35D2B}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3028,10 +3028,10 @@
         <v>0.28299999999999997</v>
       </c>
       <c r="D7" s="3">
-        <v>21.4</v>
+        <v>21.3</v>
       </c>
       <c r="E7" s="3">
-        <v>21.4</v>
+        <v>21.3</v>
       </c>
       <c r="F7" s="2">
         <v>6.0000000000000001E-3</v>
@@ -3063,10 +3063,10 @@
         <v>0.32200000000000001</v>
       </c>
       <c r="D8" s="3">
-        <v>20.100000000000001</v>
+        <v>20</v>
       </c>
       <c r="E8" s="3">
-        <v>20.100000000000001</v>
+        <v>20</v>
       </c>
       <c r="F8" s="2">
         <v>6.0000000000000001E-3</v>
@@ -3098,10 +3098,10 @@
         <v>0.33600000000000002</v>
       </c>
       <c r="D9" s="3">
-        <v>20.7</v>
+        <v>20.6</v>
       </c>
       <c r="E9" s="3">
-        <v>20.7</v>
+        <v>20.6</v>
       </c>
       <c r="F9" s="2">
         <v>6.0000000000000001E-3</v>
@@ -3121,6 +3121,78 @@
       <c r="K9" s="3">
         <v>15.3</v>
       </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="5"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="5"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="5"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="5"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="5"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="5"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="5"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="5"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="5"/>
+      <c r="B33" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>